<commit_message>
final wokring product w/o style
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -903,40 +903,40 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>33086.83</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>33397.95</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>33836.51</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>34258.23</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>34600.35</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>34811.8</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>35099.67</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>35287.45</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>35509.63</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>35575.43</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>35812.37</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>36032.84</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -944,40 +944,40 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>-19778703</v>
+        <v>-598</v>
       </c>
       <c r="C3">
-        <v>-23706509</v>
+        <v>-710</v>
       </c>
       <c r="D3">
-        <v>-23969987</v>
+        <v>-708</v>
       </c>
       <c r="E3">
-        <v>-14443124</v>
+        <v>-422</v>
       </c>
       <c r="F3">
-        <v>-21126040</v>
+        <v>-611</v>
       </c>
       <c r="G3">
-        <v>-15444643</v>
+        <v>-444</v>
       </c>
       <c r="H3">
-        <v>-17923877</v>
+        <v>-511</v>
       </c>
       <c r="I3">
-        <v>-21546547</v>
+        <v>-611</v>
       </c>
       <c r="J3">
-        <v>-18259411</v>
+        <v>-514</v>
       </c>
       <c r="K3">
-        <v>-18616873</v>
+        <v>-523</v>
       </c>
       <c r="L3">
-        <v>-23615784</v>
+        <v>-659</v>
       </c>
       <c r="M3">
-        <v>-13020231</v>
+        <v>-361</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -985,40 +985,40 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>-2449313</v>
+        <v>-74</v>
       </c>
       <c r="C4">
-        <v>-3303871</v>
+        <v>-99</v>
       </c>
       <c r="D4">
-        <v>-3074060</v>
+        <v>-91</v>
       </c>
       <c r="E4">
-        <v>-2495352</v>
+        <v>-73</v>
       </c>
       <c r="F4">
-        <v>-8423135</v>
+        <v>-243</v>
       </c>
       <c r="G4">
-        <v>-2578859</v>
+        <v>-74</v>
       </c>
       <c r="H4">
-        <v>-2221514</v>
+        <v>-63</v>
       </c>
       <c r="I4">
-        <v>-1846619</v>
+        <v>-52</v>
       </c>
       <c r="J4">
-        <v>-2234514</v>
+        <v>-63</v>
       </c>
       <c r="K4">
-        <v>-6821369</v>
+        <v>-192</v>
       </c>
       <c r="L4">
-        <v>-1755750</v>
+        <v>-49</v>
       </c>
       <c r="M4">
-        <v>-1540536</v>
+        <v>-43</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1026,40 +1026,40 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>-1403503</v>
+        <v>-42</v>
       </c>
       <c r="C5">
-        <v>-984824</v>
+        <v>-29</v>
       </c>
       <c r="D5">
-        <v>-3950541</v>
+        <v>-117</v>
       </c>
       <c r="E5">
-        <v>275731</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>-1804967</v>
+        <v>-52</v>
       </c>
       <c r="G5">
-        <v>-2603924</v>
+        <v>-75</v>
       </c>
       <c r="H5">
-        <v>-3734820</v>
+        <v>-106</v>
       </c>
       <c r="I5">
-        <v>-2966444</v>
+        <v>-84</v>
       </c>
       <c r="J5">
-        <v>-4727362</v>
+        <v>-133</v>
       </c>
       <c r="K5">
-        <v>-5700827</v>
+        <v>-160</v>
       </c>
       <c r="L5">
-        <v>-4152179</v>
+        <v>-116</v>
       </c>
       <c r="M5">
-        <v>-4457619</v>
+        <v>-124</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1067,40 +1067,40 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>-16018692</v>
+        <v>-484</v>
       </c>
       <c r="C6">
-        <v>-36362968</v>
+        <v>-1089</v>
       </c>
       <c r="D6">
-        <v>3224916</v>
+        <v>95</v>
       </c>
       <c r="E6">
-        <v>-11644409</v>
+        <v>-340</v>
       </c>
       <c r="F6">
-        <v>-16681938</v>
+        <v>-482</v>
       </c>
       <c r="G6">
-        <v>-31567102</v>
+        <v>-907</v>
       </c>
       <c r="H6">
-        <v>-51303115</v>
+        <v>-1462</v>
       </c>
       <c r="I6">
-        <v>-18025419</v>
+        <v>-511</v>
       </c>
       <c r="J6">
-        <v>-14436872</v>
+        <v>-407</v>
       </c>
       <c r="K6">
-        <v>-17161721</v>
+        <v>-482</v>
       </c>
       <c r="L6">
-        <v>-19457318</v>
+        <v>-543</v>
       </c>
       <c r="M6">
-        <v>-5939970</v>
+        <v>-165</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1108,40 +1108,40 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>-7881729</v>
+        <v>-238</v>
       </c>
       <c r="C7">
-        <v>-4175440</v>
+        <v>-125</v>
       </c>
       <c r="D7">
-        <v>-5037823</v>
+        <v>-149</v>
       </c>
       <c r="E7">
-        <v>-7763518</v>
+        <v>-227</v>
       </c>
       <c r="F7">
-        <v>-3270089</v>
+        <v>-95</v>
       </c>
       <c r="G7">
-        <v>-18102485</v>
+        <v>-520</v>
       </c>
       <c r="H7">
-        <v>-12691881</v>
+        <v>-362</v>
       </c>
       <c r="I7">
-        <v>-7858168</v>
+        <v>-223</v>
       </c>
       <c r="J7">
-        <v>-1286593</v>
+        <v>-36</v>
       </c>
       <c r="K7">
-        <v>-7015097</v>
+        <v>-197</v>
       </c>
       <c r="L7">
-        <v>-7747421</v>
+        <v>-216</v>
       </c>
       <c r="M7">
-        <v>-7809322</v>
+        <v>-217</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1149,40 +1149,40 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>-3215670</v>
+        <v>-97</v>
       </c>
       <c r="C8">
-        <v>-2812650</v>
+        <v>-84</v>
       </c>
       <c r="D8">
-        <v>-3433215</v>
+        <v>-101</v>
       </c>
       <c r="E8">
-        <v>-4719009</v>
+        <v>-138</v>
       </c>
       <c r="F8">
-        <v>-5560501</v>
+        <v>-161</v>
       </c>
       <c r="G8">
-        <v>-4745655</v>
+        <v>-136</v>
       </c>
       <c r="H8">
-        <v>-9476099</v>
+        <v>-270</v>
       </c>
       <c r="I8">
-        <v>-5028764</v>
+        <v>-143</v>
       </c>
       <c r="J8">
-        <v>-2409465</v>
+        <v>-68</v>
       </c>
       <c r="K8">
-        <v>-1538161</v>
+        <v>-43</v>
       </c>
       <c r="L8">
-        <v>529582</v>
+        <v>15</v>
       </c>
       <c r="M8">
-        <v>-847070</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1190,40 +1190,40 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>-2326999</v>
+        <v>-70</v>
       </c>
       <c r="C9">
-        <v>-3855856</v>
+        <v>-115</v>
       </c>
       <c r="D9">
-        <v>-4387399</v>
+        <v>-130</v>
       </c>
       <c r="E9">
-        <v>-4850426</v>
+        <v>-142</v>
       </c>
       <c r="F9">
-        <v>-4467989</v>
+        <v>-129</v>
       </c>
       <c r="G9">
-        <v>-5393937</v>
+        <v>-155</v>
       </c>
       <c r="H9">
-        <v>-6787511</v>
+        <v>-193</v>
       </c>
       <c r="I9">
-        <v>-5236837</v>
+        <v>-148</v>
       </c>
       <c r="J9">
-        <v>-4824557</v>
+        <v>-136</v>
       </c>
       <c r="K9">
-        <v>-5317999</v>
+        <v>-149</v>
       </c>
       <c r="L9">
-        <v>-5509924</v>
+        <v>-154</v>
       </c>
       <c r="M9">
-        <v>-5959167</v>
+        <v>-165</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1231,40 +1231,40 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>-50747610</v>
+        <v>-1533</v>
       </c>
       <c r="C10">
-        <v>-71346262</v>
+        <v>-2136</v>
       </c>
       <c r="D10">
-        <v>-36240710</v>
+        <v>-1071</v>
       </c>
       <c r="E10">
-        <v>-40789681</v>
+        <v>-1192</v>
       </c>
       <c r="F10">
-        <v>-56866670</v>
+        <v>-1644</v>
       </c>
       <c r="G10">
-        <v>-75042668</v>
+        <v>-2156</v>
       </c>
       <c r="H10">
-        <v>-97351306</v>
+        <v>-2774</v>
       </c>
       <c r="I10">
-        <v>-57271961</v>
+        <v>-1624</v>
       </c>
       <c r="J10">
-        <v>-43354217</v>
+        <v>-1221</v>
       </c>
       <c r="K10">
-        <v>-56854048</v>
+        <v>-1597</v>
       </c>
       <c r="L10">
-        <v>-56198870</v>
+        <v>-1568</v>
       </c>
       <c r="M10">
-        <v>-33614748</v>
+        <v>-934</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1272,40 +1272,40 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>-53074609</v>
+        <v>-1603</v>
       </c>
       <c r="C11">
-        <v>-75202118</v>
+        <v>-2251</v>
       </c>
       <c r="D11">
-        <v>-40628109</v>
+        <v>-1201</v>
       </c>
       <c r="E11">
-        <v>-45640107</v>
+        <v>-1334</v>
       </c>
       <c r="F11">
-        <v>-61334659</v>
+        <v>-1773</v>
       </c>
       <c r="G11">
-        <v>-80436605</v>
+        <v>-2311</v>
       </c>
       <c r="H11">
-        <v>-104138817</v>
+        <v>-2967</v>
       </c>
       <c r="I11">
-        <v>-62508798</v>
+        <v>-1772</v>
       </c>
       <c r="J11">
-        <v>-48178774</v>
+        <v>-1357</v>
       </c>
       <c r="K11">
-        <v>-62172047</v>
+        <v>-1746</v>
       </c>
       <c r="L11">
-        <v>-61708794</v>
+        <v>-1722</v>
       </c>
       <c r="M11">
-        <v>-39573915</v>
+        <v>-1099</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1313,28 +1313,28 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>-6907071</v>
+        <v>-209</v>
       </c>
       <c r="C12">
-        <v>-6890680</v>
+        <v>-206</v>
       </c>
       <c r="D12">
         <v>-0</v>
       </c>
       <c r="E12">
-        <v>-7259745</v>
+        <v>-212</v>
       </c>
       <c r="F12">
         <v>-0</v>
       </c>
       <c r="G12">
-        <v>-7259745</v>
+        <v>-209</v>
       </c>
       <c r="H12">
-        <v>-3103243</v>
+        <v>-88</v>
       </c>
       <c r="I12">
-        <v>-1569786</v>
+        <v>-44</v>
       </c>
       <c r="J12">
         <v>-0</v>
@@ -1343,10 +1343,10 @@
         <v>-0</v>
       </c>
       <c r="L12">
-        <v>-10678625</v>
+        <v>-298</v>
       </c>
       <c r="M12">
-        <v>-107274</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1354,40 +1354,40 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>-1822097</v>
+        <v>-55</v>
       </c>
       <c r="C13">
-        <v>-1822097</v>
+        <v>-55</v>
       </c>
       <c r="D13">
-        <v>-1822097</v>
+        <v>-54</v>
       </c>
       <c r="E13">
-        <v>-1822097</v>
+        <v>-53</v>
       </c>
       <c r="F13">
-        <v>-1822097</v>
+        <v>-53</v>
       </c>
       <c r="G13">
-        <v>-1822097</v>
+        <v>-52</v>
       </c>
       <c r="H13">
-        <v>-1822097</v>
+        <v>-52</v>
       </c>
       <c r="I13">
-        <v>-1803662</v>
+        <v>-51</v>
       </c>
       <c r="J13">
-        <v>-1845504</v>
+        <v>-52</v>
       </c>
       <c r="K13">
-        <v>-1824524</v>
+        <v>-51</v>
       </c>
       <c r="L13">
-        <v>-1824524</v>
+        <v>-51</v>
       </c>
       <c r="M13">
-        <v>-1824524</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1395,40 +1395,40 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>-1695671</v>
+        <v>-51</v>
       </c>
       <c r="C14">
-        <v>-1818098</v>
+        <v>-54</v>
       </c>
       <c r="D14">
-        <v>-2005362</v>
+        <v>-59</v>
       </c>
       <c r="E14">
-        <v>-2247605</v>
+        <v>-66</v>
       </c>
       <c r="F14">
-        <v>-2405379</v>
+        <v>-70</v>
       </c>
       <c r="G14">
-        <v>-2666738</v>
+        <v>-77</v>
       </c>
       <c r="H14">
-        <v>-3289733</v>
+        <v>-94</v>
       </c>
       <c r="I14">
-        <v>-2599965</v>
+        <v>-74</v>
       </c>
       <c r="J14">
-        <v>-2563820</v>
+        <v>-72</v>
       </c>
       <c r="K14">
-        <v>-2315284</v>
+        <v>-65</v>
       </c>
       <c r="L14">
-        <v>-2650139</v>
+        <v>-74</v>
       </c>
       <c r="M14">
-        <v>-3195754</v>
+        <v>-89</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1436,40 +1436,40 @@
         <v>25</v>
       </c>
       <c r="B15">
-        <v>-10424839</v>
+        <v>-315</v>
       </c>
       <c r="C15">
-        <v>-10530875</v>
+        <v>-315</v>
       </c>
       <c r="D15">
-        <v>-3827459</v>
+        <v>-113</v>
       </c>
       <c r="E15">
-        <v>-11329447</v>
+        <v>-331</v>
       </c>
       <c r="F15">
-        <v>-4227476</v>
+        <v>-123</v>
       </c>
       <c r="G15">
-        <v>-11748580</v>
+        <v>-338</v>
       </c>
       <c r="H15">
-        <v>-8215073</v>
+        <v>-234</v>
       </c>
       <c r="I15">
-        <v>-5973413</v>
+        <v>-169</v>
       </c>
       <c r="J15">
-        <v>-4409324</v>
+        <v>-124</v>
       </c>
       <c r="K15">
-        <v>-4139808</v>
+        <v>-116</v>
       </c>
       <c r="L15">
-        <v>-15153288</v>
+        <v>-423</v>
       </c>
       <c r="M15">
-        <v>-5127552</v>
+        <v>-143</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1477,40 +1477,40 @@
         <v>26</v>
       </c>
       <c r="B16">
-        <v>114966684</v>
+        <v>3475</v>
       </c>
       <c r="C16">
-        <v>114966684</v>
+        <v>3442</v>
       </c>
       <c r="D16">
-        <v>114966684</v>
+        <v>3398</v>
       </c>
       <c r="E16">
-        <v>114966684</v>
+        <v>3356</v>
       </c>
       <c r="F16">
-        <v>114966684</v>
+        <v>3323</v>
       </c>
       <c r="G16">
-        <v>114966684</v>
+        <v>3303</v>
       </c>
       <c r="H16">
-        <v>114966684</v>
+        <v>3275</v>
       </c>
       <c r="I16">
-        <v>171258789</v>
+        <v>4853</v>
       </c>
       <c r="J16">
-        <v>171258789</v>
+        <v>4823</v>
       </c>
       <c r="K16">
-        <v>171258789</v>
+        <v>4814</v>
       </c>
       <c r="L16">
-        <v>171258789</v>
+        <v>4782</v>
       </c>
       <c r="M16">
-        <v>171258789</v>
+        <v>4753</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1518,40 +1518,40 @@
         <v>27</v>
       </c>
       <c r="B17">
-        <v>3976114</v>
+        <v>120</v>
       </c>
       <c r="C17">
-        <v>10021173</v>
+        <v>300</v>
       </c>
       <c r="D17">
-        <v>7293025</v>
+        <v>216</v>
       </c>
       <c r="E17">
-        <v>7321180</v>
+        <v>214</v>
       </c>
       <c r="F17">
-        <v>15702297</v>
+        <v>454</v>
       </c>
       <c r="G17">
-        <v>8245520</v>
+        <v>237</v>
       </c>
       <c r="H17">
-        <v>31557629</v>
+        <v>899</v>
       </c>
       <c r="I17">
-        <v>-31319150</v>
+        <v>-888</v>
       </c>
       <c r="J17">
-        <v>-28454491</v>
+        <v>-801</v>
       </c>
       <c r="K17">
-        <v>-26222842</v>
+        <v>-737</v>
       </c>
       <c r="L17">
-        <v>-25979626</v>
+        <v>-725</v>
       </c>
       <c r="M17">
-        <v>-44080324</v>
+        <v>-1223</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1559,40 +1559,40 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>-48563739</v>
+        <v>-1468</v>
       </c>
       <c r="C18">
-        <v>-44911835</v>
+        <v>-1345</v>
       </c>
       <c r="D18">
-        <v>-39931994</v>
+        <v>-1180</v>
       </c>
       <c r="E18">
-        <v>-33259545</v>
+        <v>-971</v>
       </c>
       <c r="F18">
-        <v>-26550772</v>
+        <v>-767</v>
       </c>
       <c r="G18">
-        <v>-18944955</v>
+        <v>-544</v>
       </c>
       <c r="H18">
-        <v>-22438314</v>
+        <v>-639</v>
       </c>
       <c r="I18">
-        <v>-35610381</v>
+        <v>-1009</v>
       </c>
       <c r="J18">
-        <v>-45564316</v>
+        <v>-1283</v>
       </c>
       <c r="K18">
-        <v>-35978501</v>
+        <v>-1011</v>
       </c>
       <c r="L18">
-        <v>-37349605</v>
+        <v>-1043</v>
       </c>
       <c r="M18">
-        <v>-16290029</v>
+        <v>-452</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1600,40 +1600,40 @@
         <v>29</v>
       </c>
       <c r="B19">
-        <v>-3613578</v>
+        <v>-109</v>
       </c>
       <c r="C19">
-        <v>-9671304</v>
+        <v>-290</v>
       </c>
       <c r="D19">
-        <v>-4301349</v>
+        <v>-127</v>
       </c>
       <c r="E19">
-        <v>-2062819</v>
+        <v>-60</v>
       </c>
       <c r="F19">
-        <v>-10402912</v>
+        <v>-301</v>
       </c>
       <c r="G19">
-        <v>-1159977</v>
+        <v>-33</v>
       </c>
       <c r="H19">
-        <v>-1371819</v>
+        <v>-39</v>
       </c>
       <c r="I19">
-        <v>-7133347</v>
+        <v>-202</v>
       </c>
       <c r="J19">
-        <v>-6984272</v>
+        <v>-197</v>
       </c>
       <c r="K19">
-        <v>-9793572</v>
+        <v>-275</v>
       </c>
       <c r="L19">
-        <v>-8502665</v>
+        <v>-237</v>
       </c>
       <c r="M19">
-        <v>-4077450</v>
+        <v>-113</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1641,40 +1641,40 @@
         <v>30</v>
       </c>
       <c r="B20">
-        <v>-1635754</v>
+        <v>-49</v>
       </c>
       <c r="C20">
-        <v>-1635754</v>
+        <v>-49</v>
       </c>
       <c r="D20">
-        <v>-1635754</v>
+        <v>-48</v>
       </c>
       <c r="E20">
-        <v>-1635754</v>
+        <v>-48</v>
       </c>
       <c r="F20">
-        <v>-1635754</v>
+        <v>-47</v>
       </c>
       <c r="G20">
-        <v>-1635754</v>
+        <v>-47</v>
       </c>
       <c r="H20">
-        <v>-1635754</v>
+        <v>-47</v>
       </c>
       <c r="I20">
-        <v>-2305032</v>
+        <v>-65</v>
       </c>
       <c r="J20">
-        <v>-1638344</v>
+        <v>-46</v>
       </c>
       <c r="K20">
-        <v>-1638344</v>
+        <v>-46</v>
       </c>
       <c r="L20">
-        <v>-720690</v>
+        <v>-20</v>
       </c>
       <c r="M20">
-        <v>-1387377</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1700,22 +1700,22 @@
         <v>-0</v>
       </c>
       <c r="H21">
-        <v>-4973984</v>
+        <v>-142</v>
       </c>
       <c r="I21">
-        <v>-4246174</v>
+        <v>-120</v>
       </c>
       <c r="J21">
-        <v>-10559357</v>
+        <v>-297</v>
       </c>
       <c r="K21">
-        <v>9220158</v>
+        <v>259</v>
       </c>
       <c r="L21">
         <v>-0</v>
       </c>
       <c r="M21">
-        <v>-13786568</v>
+        <v>-383</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1723,40 +1723,40 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>65129727</v>
+        <v>1969</v>
       </c>
       <c r="C22">
-        <v>68768964</v>
+        <v>2058</v>
       </c>
       <c r="D22">
-        <v>76390612</v>
+        <v>2259</v>
       </c>
       <c r="E22">
-        <v>85329746</v>
+        <v>2491</v>
       </c>
       <c r="F22">
-        <v>92079543</v>
+        <v>2662</v>
       </c>
       <c r="G22">
-        <v>101471518</v>
+        <v>2916</v>
       </c>
       <c r="H22">
-        <v>116104442</v>
+        <v>3307</v>
       </c>
       <c r="I22">
-        <v>90644705</v>
+        <v>2569</v>
       </c>
       <c r="J22">
-        <v>78058009</v>
+        <v>2199</v>
       </c>
       <c r="K22">
-        <v>106845688</v>
+        <v>3004</v>
       </c>
       <c r="L22">
-        <v>98706203</v>
+        <v>2757</v>
       </c>
       <c r="M22">
-        <v>91637041</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1764,40 +1764,40 @@
         <v>33</v>
       </c>
       <c r="B23">
-        <v>109853</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>463186</v>
+        <v>14</v>
       </c>
       <c r="D23">
-        <v>45114</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>283870</v>
+        <v>8</v>
       </c>
       <c r="F23">
-        <v>168265</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>171316</v>
+        <v>5</v>
       </c>
       <c r="H23">
-        <v>239939</v>
+        <v>7</v>
       </c>
       <c r="I23">
-        <v>516729</v>
+        <v>15</v>
       </c>
       <c r="J23">
-        <v>199974</v>
+        <v>6</v>
       </c>
       <c r="K23">
-        <v>684778</v>
+        <v>19</v>
       </c>
       <c r="L23">
-        <v>400802</v>
+        <v>11</v>
       </c>
       <c r="M23">
-        <v>237873</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1805,40 +1805,40 @@
         <v>34</v>
       </c>
       <c r="B24">
-        <v>109853</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>463186</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>45114</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>283870</v>
+        <v>8</v>
       </c>
       <c r="F24">
-        <v>168265</v>
+        <v>5</v>
       </c>
       <c r="G24">
-        <v>171316</v>
+        <v>5</v>
       </c>
       <c r="H24">
-        <v>239939</v>
+        <v>7</v>
       </c>
       <c r="I24">
-        <v>516729</v>
+        <v>15</v>
       </c>
       <c r="J24">
-        <v>199974</v>
+        <v>6</v>
       </c>
       <c r="K24">
-        <v>684778</v>
+        <v>19</v>
       </c>
       <c r="L24">
-        <v>400802</v>
+        <v>11</v>
       </c>
       <c r="M24">
-        <v>237873</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1846,40 +1846,40 @@
         <v>35</v>
       </c>
       <c r="B25">
-        <v>65239580</v>
+        <v>1972</v>
       </c>
       <c r="C25">
-        <v>69232150</v>
+        <v>2072</v>
       </c>
       <c r="D25">
-        <v>76435726</v>
+        <v>2260</v>
       </c>
       <c r="E25">
-        <v>85613616</v>
+        <v>2499</v>
       </c>
       <c r="F25">
-        <v>92247808</v>
+        <v>2667</v>
       </c>
       <c r="G25">
-        <v>101642834</v>
+        <v>2921</v>
       </c>
       <c r="H25">
-        <v>116344381</v>
+        <v>3314</v>
       </c>
       <c r="I25">
-        <v>91161434</v>
+        <v>2584</v>
       </c>
       <c r="J25">
-        <v>78257983</v>
+        <v>2205</v>
       </c>
       <c r="K25">
-        <v>107530466</v>
+        <v>3023</v>
       </c>
       <c r="L25">
-        <v>99107005</v>
+        <v>2768</v>
       </c>
       <c r="M25">
-        <v>91874914</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1887,40 +1887,40 @@
         <v>36</v>
       </c>
       <c r="B26">
-        <v>2410781</v>
+        <v>73</v>
       </c>
       <c r="C26">
-        <v>2813731</v>
+        <v>84</v>
       </c>
       <c r="D26">
-        <v>3005001</v>
+        <v>89</v>
       </c>
       <c r="E26">
-        <v>3363566</v>
+        <v>98</v>
       </c>
       <c r="F26">
-        <v>3381590</v>
+        <v>98</v>
       </c>
       <c r="G26">
-        <v>3479147</v>
+        <v>100</v>
       </c>
       <c r="H26">
-        <v>4267043</v>
+        <v>122</v>
       </c>
       <c r="I26">
-        <v>3359813</v>
+        <v>95</v>
       </c>
       <c r="J26">
-        <v>2309868</v>
+        <v>65</v>
       </c>
       <c r="K26">
-        <v>2553922</v>
+        <v>72</v>
       </c>
       <c r="L26">
-        <v>1822762</v>
+        <v>51</v>
       </c>
       <c r="M26">
-        <v>1937742</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1931,37 +1931,37 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>39847</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>45461</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>46018</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>53031</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <v>97227</v>
+        <v>3</v>
       </c>
       <c r="H27">
-        <v>97821</v>
+        <v>3</v>
       </c>
       <c r="I27">
-        <v>81835</v>
+        <v>2</v>
       </c>
       <c r="J27">
-        <v>51167</v>
+        <v>1</v>
       </c>
       <c r="K27">
-        <v>186638</v>
+        <v>5</v>
       </c>
       <c r="L27">
-        <v>148706</v>
+        <v>4</v>
       </c>
       <c r="M27">
-        <v>97875</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1969,40 +1969,40 @@
         <v>38</v>
       </c>
       <c r="B28">
-        <v>176497</v>
+        <v>5</v>
       </c>
       <c r="C28">
-        <v>638191</v>
+        <v>19</v>
       </c>
       <c r="D28">
-        <v>728280</v>
+        <v>22</v>
       </c>
       <c r="E28">
-        <v>880994</v>
+        <v>26</v>
       </c>
       <c r="F28">
-        <v>532742</v>
+        <v>15</v>
       </c>
       <c r="G28">
-        <v>1450332</v>
+        <v>42</v>
       </c>
       <c r="H28">
-        <v>932103</v>
+        <v>27</v>
       </c>
       <c r="I28">
-        <v>903165</v>
+        <v>26</v>
       </c>
       <c r="J28">
-        <v>815064</v>
+        <v>23</v>
       </c>
       <c r="K28">
-        <v>780640</v>
+        <v>22</v>
       </c>
       <c r="L28">
-        <v>4927090</v>
+        <v>138</v>
       </c>
       <c r="M28">
-        <v>6346508</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2092,40 +2092,40 @@
         <v>41</v>
       </c>
       <c r="B31">
-        <v>2587278</v>
+        <v>78</v>
       </c>
       <c r="C31">
-        <v>3491769</v>
+        <v>104</v>
       </c>
       <c r="D31">
-        <v>3778742</v>
+        <v>112</v>
       </c>
       <c r="E31">
-        <v>4290578</v>
+        <v>125</v>
       </c>
       <c r="F31">
-        <v>3967363</v>
+        <v>115</v>
       </c>
       <c r="G31">
-        <v>5026706</v>
+        <v>145</v>
       </c>
       <c r="H31">
-        <v>5296967</v>
+        <v>152</v>
       </c>
       <c r="I31">
-        <v>4344813</v>
+        <v>123</v>
       </c>
       <c r="J31">
-        <v>3176099</v>
+        <v>89</v>
       </c>
       <c r="K31">
-        <v>3521200</v>
+        <v>99</v>
       </c>
       <c r="L31">
-        <v>6898558</v>
+        <v>193</v>
       </c>
       <c r="M31">
-        <v>8382125</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2133,40 +2133,40 @@
         <v>42</v>
       </c>
       <c r="B32">
-        <v>15063769</v>
+        <v>455</v>
       </c>
       <c r="C32">
-        <v>19286684</v>
+        <v>577</v>
       </c>
       <c r="D32">
-        <v>23715132</v>
+        <v>701</v>
       </c>
       <c r="E32">
-        <v>24049505</v>
+        <v>702</v>
       </c>
       <c r="F32">
-        <v>23964767</v>
+        <v>693</v>
       </c>
       <c r="G32">
-        <v>22264572</v>
+        <v>640</v>
       </c>
       <c r="H32">
-        <v>31292841</v>
+        <v>892</v>
       </c>
       <c r="I32">
-        <v>23298834</v>
+        <v>660</v>
       </c>
       <c r="J32">
-        <v>20808167</v>
+        <v>586</v>
       </c>
       <c r="K32">
-        <v>22841974</v>
+        <v>642</v>
       </c>
       <c r="L32">
-        <v>22384606</v>
+        <v>625</v>
       </c>
       <c r="M32">
-        <v>23768434</v>
+        <v>660</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2297,40 +2297,40 @@
         <v>46</v>
       </c>
       <c r="B36">
-        <v>15063769</v>
+        <v>455</v>
       </c>
       <c r="C36">
-        <v>19286684</v>
+        <v>577</v>
       </c>
       <c r="D36">
-        <v>23715132</v>
+        <v>701</v>
       </c>
       <c r="E36">
-        <v>24049505</v>
+        <v>702</v>
       </c>
       <c r="F36">
-        <v>23964767</v>
+        <v>693</v>
       </c>
       <c r="G36">
-        <v>22264572</v>
+        <v>640</v>
       </c>
       <c r="H36">
-        <v>31292841</v>
+        <v>892</v>
       </c>
       <c r="I36">
-        <v>23298834</v>
+        <v>660</v>
       </c>
       <c r="J36">
-        <v>20808167</v>
+        <v>586</v>
       </c>
       <c r="K36">
-        <v>22841974</v>
+        <v>642</v>
       </c>
       <c r="L36">
-        <v>22384606</v>
+        <v>625</v>
       </c>
       <c r="M36">
-        <v>23768434</v>
+        <v>660</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2338,40 +2338,40 @@
         <v>47</v>
       </c>
       <c r="B37">
-        <v>82890627</v>
+        <v>2505</v>
       </c>
       <c r="C37">
-        <v>92010603</v>
+        <v>2753</v>
       </c>
       <c r="D37">
-        <v>103929600</v>
+        <v>3073</v>
       </c>
       <c r="E37">
-        <v>113953699</v>
+        <v>3326</v>
       </c>
       <c r="F37">
-        <v>120179938</v>
+        <v>3475</v>
       </c>
       <c r="G37">
-        <v>128934112</v>
+        <v>3706</v>
       </c>
       <c r="H37">
-        <v>152934189</v>
+        <v>4358</v>
       </c>
       <c r="I37">
-        <v>118805081</v>
+        <v>3367</v>
       </c>
       <c r="J37">
-        <v>102242249</v>
+        <v>2880</v>
       </c>
       <c r="K37">
-        <v>133893640</v>
+        <v>3764</v>
       </c>
       <c r="L37">
-        <v>128390169</v>
+        <v>3586</v>
       </c>
       <c r="M37">
-        <v>124025473</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="38" spans="1:13">

</xml_diff>